<commit_message>
resize in photoshop script
</commit_message>
<xml_diff>
--- a/nominal_position.xlsx
+++ b/nominal_position.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\PycharmProjects\montager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C381BEAC-5B07-4A56-95E6-99227DC47DEC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{35EC1FD8-4333-4DAA-9E9F-CC6F8A4E7743}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,61 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="77">
-  <si>
-    <t>0000</t>
-  </si>
-  <si>
-    <t>TRC</t>
-  </si>
-  <si>
-    <t>0001</t>
-  </si>
-  <si>
-    <t>MRE</t>
-  </si>
-  <si>
-    <t>0002</t>
-  </si>
-  <si>
-    <t>BRC</t>
-  </si>
-  <si>
-    <t>0003</t>
-  </si>
-  <si>
-    <t>MBE</t>
-  </si>
-  <si>
-    <t>0004</t>
-  </si>
-  <si>
-    <t>BLC</t>
-  </si>
-  <si>
-    <t>0005</t>
-  </si>
-  <si>
-    <t>MLE</t>
-  </si>
-  <si>
-    <t>0006</t>
-  </si>
-  <si>
-    <t>TLC</t>
-  </si>
-  <si>
-    <t>0007</t>
-  </si>
-  <si>
-    <t>MTE</t>
-  </si>
-  <si>
-    <t>0008</t>
-  </si>
-  <si>
-    <t>CENTRE</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="59">
   <si>
     <t>0009</t>
   </si>
@@ -616,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -632,7 +578,7 @@
         <v>1</v>
       </c>
       <c r="C1">
-        <v>0.7</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -643,7 +589,7 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>0.7</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -651,84 +597,84 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3">
-        <v>0.7</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="C4">
-        <v>0.7</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5">
-        <v>0.7</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6">
-        <v>0.7</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7">
-        <v>0.7</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C8">
-        <v>0.7</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="C9">
-        <v>0.7</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C10">
         <v>1.5</v>
@@ -736,10 +682,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C11">
         <v>1.5</v>
@@ -747,10 +693,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C12">
         <v>1.5</v>
@@ -758,10 +704,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>76</v>
+        <v>3</v>
       </c>
       <c r="C13">
         <v>1.5</v>
@@ -769,10 +715,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C14">
         <v>1.5</v>
@@ -780,10 +726,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C15">
         <v>1.5</v>
@@ -791,10 +737,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="C16">
         <v>1.5</v>
@@ -802,7 +748,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
         <v>25</v>
@@ -813,10 +759,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>76</v>
+        <v>27</v>
       </c>
       <c r="C18">
         <v>1.5</v>
@@ -824,10 +770,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C19">
         <v>1.5</v>
@@ -835,10 +781,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="C20">
         <v>1.5</v>
@@ -846,10 +792,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="C21">
         <v>1.5</v>
@@ -857,10 +803,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C22">
         <v>1.5</v>
@@ -868,10 +814,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C23">
         <v>1.5</v>
@@ -879,10 +825,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="C24">
         <v>1.5</v>
@@ -890,10 +836,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C25">
         <v>1.5</v>
@@ -901,10 +847,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="C26">
         <v>1.5</v>
@@ -912,10 +858,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="C27">
         <v>1.5</v>
@@ -923,10 +869,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B28" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="C28">
         <v>1.5</v>
@@ -934,10 +880,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B29" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="C29">
         <v>1.5</v>
@@ -945,10 +891,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B30" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="C30">
         <v>1.5</v>
@@ -956,10 +902,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B31" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C31">
         <v>1.5</v>
@@ -967,10 +913,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B32" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C32">
         <v>1.5</v>
@@ -978,10 +924,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B33" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="C33">
         <v>1.5</v>
@@ -989,10 +935,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B34" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="C34">
         <v>1.5</v>
@@ -1000,10 +946,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B35" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="C35">
         <v>1.5</v>
@@ -1011,10 +957,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B36" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="C36">
         <v>1.5</v>
@@ -1022,111 +968,12 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B37" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="C37">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>59</v>
-      </c>
-      <c r="B38" t="s">
-        <v>60</v>
-      </c>
-      <c r="C38">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>61</v>
-      </c>
-      <c r="B39" t="s">
-        <v>62</v>
-      </c>
-      <c r="C39">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>63</v>
-      </c>
-      <c r="B40" t="s">
-        <v>64</v>
-      </c>
-      <c r="C40">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>65</v>
-      </c>
-      <c r="B41" t="s">
-        <v>66</v>
-      </c>
-      <c r="C41">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>67</v>
-      </c>
-      <c r="B42" t="s">
-        <v>68</v>
-      </c>
-      <c r="C42">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>69</v>
-      </c>
-      <c r="B43" t="s">
-        <v>70</v>
-      </c>
-      <c r="C43">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>71</v>
-      </c>
-      <c r="B44" t="s">
-        <v>72</v>
-      </c>
-      <c r="C44">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>73</v>
-      </c>
-      <c r="B45" t="s">
-        <v>74</v>
-      </c>
-      <c r="C45">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>75</v>
-      </c>
-      <c r="B46" t="s">
-        <v>74</v>
-      </c>
-      <c r="C46">
         <v>1.5</v>
       </c>
     </row>

</xml_diff>